<commit_message>
Added excel spreadsheet model
</commit_message>
<xml_diff>
--- a/data-preproc/aws_pipelines.xlsx
+++ b/data-preproc/aws_pipelines.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Pipeline Name</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Cores used</t>
-  </si>
-  <si>
-    <t>Number of nodes</t>
   </si>
   <si>
     <t>CPAC</t>
@@ -83,6 +80,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -104,6 +102,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,7 +176,7 @@
   <dimension ref="A2:J20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -219,13 +218,11 @@
       <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.055</v>
@@ -243,7 +240,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>8</v>
@@ -251,7 +248,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.0071</v>
@@ -270,7 +267,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>4</v>
@@ -278,7 +275,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0.0071</v>
@@ -297,7 +294,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>8</v>
@@ -305,7 +302,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0.0071</v>
@@ -324,7 +321,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>8</v>
@@ -332,15 +329,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,24 +392,15 @@
       <c r="B18" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C18" s="0" t="n">
-        <v>5000</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>10000</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in the QAP numbers
</commit_message>
<xml_diff>
--- a/data-preproc/aws_pipelines.xlsx
+++ b/data-preproc/aws_pipelines.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Pipeline Name</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>ANTs</t>
+  </si>
+  <si>
+    <t>QAP</t>
+  </si>
+  <si>
+    <t>c3.4xlarge</t>
   </si>
   <si>
     <t>Run sim for:</t>
@@ -176,7 +182,7 @@
   <dimension ref="A2:J20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -327,17 +333,43 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>